<commit_message>
Added Screen Data. Added All Screen Display. Updated Migration.
</commit_message>
<xml_diff>
--- a/GameModel (1).xlsx
+++ b/GameModel (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elliot Robinson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Embry-Riddle\Visual Studio Projects\AdventureGame\Adventure-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C389FD8D-4D98-4313-9D97-9F954D017FD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450DE042-B70D-4A4F-B640-23762EC5C1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A256BCB-D528-4AE6-81E3-6DAAD0301137}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{9A256BCB-D528-4AE6-81E3-6DAAD0301137}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
   <si>
     <t>UserId</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Exp</t>
   </si>
   <si>
-    <t>Write a description for this screen, which lies directly west of 3.</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -240,6 +237,12 @@
   </si>
   <si>
     <t>snarles at you half-heartedly</t>
+  </si>
+  <si>
+    <t>Main Road2</t>
+  </si>
+  <si>
+    <t>A road to the west of the Main Road filled with holes.</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AAE58CB-0B9E-410A-B356-BCEC33F6B202}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
@@ -640,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -715,13 +718,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,7 +764,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -773,13 +776,13 @@
         <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>34</v>
@@ -790,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -816,10 +819,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -859,13 +862,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -882,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -923,10 +926,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,7 +973,7 @@
         <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39C3BFF-BEA8-4D50-966A-F8597203528B}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,10 +1067,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1075,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -1086,7 +1089,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1097,10 +1100,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,10 +1111,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1230,7 +1233,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1338,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,7 +1349,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1354,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1455,7 +1458,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>19</v>
@@ -1472,13 +1475,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added navigation to chest and key. Started on remodeling of data models
</commit_message>
<xml_diff>
--- a/GameModel (1).xlsx
+++ b/GameModel (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Embry-Riddle\Visual Studio Projects\AdventureGame\Adventure-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450DE042-B70D-4A4F-B640-23762EC5C1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDA59A1-6C2C-4104-95D6-FEAF4C6EA138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{9A256BCB-D528-4AE6-81E3-6DAAD0301137}"/>
   </bookViews>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>